<commit_message>
control player from notification(except play and pause)
</commit_message>
<xml_diff>
--- a/app/src/main/java/com/example/music/PLAN.xlsx
+++ b/app/src/main/java/com/example/music/PLAN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~project\AndroidKotlin\MUSIC\app\src\main\java\com\example\music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D5FFE6-298F-413F-975A-35E30B90E706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C383DCCF-2393-47E3-A53A-F11A8ECB6256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -793,9 +793,7 @@
       <c r="H8" s="11">
         <v>44809</v>
       </c>
-      <c r="I8" s="12">
-        <v>44075</v>
-      </c>
+      <c r="I8" s="12"/>
       <c r="J8" s="6"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>

</xml_diff>